<commit_message>
try/catch for registering item
</commit_message>
<xml_diff>
--- a/filename1.xlsx
+++ b/filename1.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -529,10 +529,180 @@
         <v>Vola alto nel cielo</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="1" t="str">
+        <v>1699920208662_Glass</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <v>Glass</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <v>Tiny</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <v>For drinking</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="str">
+        <v>1699922521471_</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="str">
+        <v>1699923027138_test</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <v>test</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="str">
+        <v>1699923083383_test</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <v>test</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E13" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="str">
+        <v>1699923106468_Test</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <v>Test</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E14" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="str">
+        <v>1699923300586_test</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <v>test</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E15" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="str">
+        <v>1699923477814_test</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <v>test</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E16" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="str">
+        <v>1699923506634_Test</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <v>Test</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E17" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="str">
+        <v>1699923598844_Prova</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <v>Prova</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E18" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="str">
+        <v>1699923635918_Prova</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <v>Prova</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E19" s="1" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>